<commit_message>
User can set derived params
</commit_message>
<xml_diff>
--- a/All_Exps.xlsx
+++ b/All_Exps.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>exp_ID</t>
   </si>
@@ -48,62 +48,50 @@
     <t>crop ID (as in crop.json)</t>
   </si>
   <si>
-    <t>GM_300</t>
-  </si>
-  <si>
-    <t>sim_1.json</t>
-  </si>
-  <si>
-    <t>crop_1.json</t>
-  </si>
-  <si>
-    <t>site_1.json</t>
-  </si>
-  <si>
-    <t>climate_padova.csv</t>
-  </si>
-  <si>
-    <t>maize_PD.json</t>
-  </si>
-  <si>
-    <t>grain maize_PD_300.json</t>
-  </si>
-  <si>
-    <t>grain maize_PD_600.json</t>
-  </si>
-  <si>
-    <t>1-2-3</t>
-  </si>
-  <si>
-    <t>GM_600</t>
-  </si>
-  <si>
-    <t>sim_2.json</t>
-  </si>
-  <si>
-    <t>crop_2.json</t>
-  </si>
-  <si>
-    <t>site_2.json</t>
+    <t>sim_WW_Samanta_DOM_2006.json</t>
+  </si>
+  <si>
+    <t>crop_WW_Samanta_DOM_2006.json</t>
+  </si>
+  <si>
+    <t>sim_WW_Samanta_DOM_2007.json</t>
+  </si>
+  <si>
+    <t>crop_WW_Samanta_DOM_2007.json</t>
+  </si>
+  <si>
+    <t>WW</t>
+  </si>
+  <si>
+    <t>dom.json</t>
+  </si>
+  <si>
+    <t>dom.csv</t>
+  </si>
+  <si>
+    <t>wheat_CZ.json</t>
+  </si>
+  <si>
+    <t>winter wheat_CZ.json</t>
+  </si>
+  <si>
+    <t>sim_WW_Samanta_DOM_2008.json</t>
+  </si>
+  <si>
+    <t>crop_WW_Samanta_DOM_2008.json</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFCCCCCC"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,10 +114,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,17 +418,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
@@ -484,122 +471,90 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>